<commit_message>
minor additions and v2.4
</commit_message>
<xml_diff>
--- a/arena_12-12/production_v2/BOM.xlsx
+++ b/arena_12-12/production_v2/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="101">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -100,45 +100,48 @@
     <t xml:space="preserve">478-8496-1-ND</t>
   </si>
   <si>
+    <t xml:space="preserve">Footprint and GERBER differ, but it should fit. Any generic capacitor with same specs is OK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC REG LINEAR 3.3V 3A 5DDPAK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5DDPAK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analog Devices Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LT1764EQ-3.3#PBF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LT1764EQ-3.3#PBF-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alternative:  LT1764EQ#TRPBF </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C3;C5;C6;C10;C12;C14;C16;C18;C19;C22;C24;C25;C26;C27;C28;C29;C30;C31;C32;C33;C34;C35;C36;C37;C41;C44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAP CER 0.1UF 50V X7R 0805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Walsin Technology Corporation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0805B104J500CT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1292-1564-1-ND</t>
+  </si>
+  <si>
     <t xml:space="preserve">Any generic capacitor with same specs is OK</t>
   </si>
   <si>
-    <t xml:space="preserve">U7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IC REG LINEAR 3.3V 3A 5DDPAK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5DDPAK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Analog Devices Inc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LT1764EQ-3.3#PBF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LT1764EQ-3.3#PBF-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alternative:  LT1764EQ#TRPBF </t>
-  </si>
-  <si>
-    <t xml:space="preserve">C3;C5;C6;C10;C12;C14;C16;C18;C19;C22;C24;C25;C26;C27;C28;C29;C30;C31;C32;C33;C34;C35;C36;C37;C41;C44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAP CER 0.1UF 50V X7R 0805</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Walsin Technology Corporation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0805B104J500CT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1292-1564-1-ND</t>
-  </si>
-  <si>
     <t xml:space="preserve">C40</t>
   </si>
   <si>
@@ -265,6 +268,9 @@
     <t xml:space="preserve">CP-102A-ND</t>
   </si>
   <si>
+    <t xml:space="preserve">Footprint of connector and GERBER differ, but it should fit. Any other connector with same specs is OK</t>
+  </si>
+  <si>
     <t xml:space="preserve">J25</t>
   </si>
   <si>
@@ -298,23 +304,7 @@
     <t xml:space="preserve">VSSR16-22-JI-ND</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Alternative: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">VSSR1603220JTF</t>
-    </r>
+    <t xml:space="preserve">Alternative: VSSR1603220JTF</t>
   </si>
   <si>
     <t xml:space="preserve">U1;U2;U3;U4;U5;U6</t>
@@ -343,7 +333,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -371,11 +361,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -460,8 +445,8 @@
   </sheetPr>
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -471,7 +456,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="81.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="53.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="6" style="1" width="53.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="1" width="53.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="86.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="1" width="53.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="34.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="51.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="11.43"/>
@@ -592,7 +579,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="n">
@@ -621,7 +608,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="n">
@@ -646,7 +633,7 @@
         <v>38</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -657,25 +644,25 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -686,25 +673,25 @@
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -715,25 +702,25 @@
         <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -744,25 +731,25 @@
         <v>2</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -773,25 +760,25 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -802,25 +789,25 @@
         <v>34</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -831,20 +818,20 @@
         <v>3</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -855,23 +842,23 @@
         <v>12</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -882,23 +869,23 @@
         <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -909,20 +896,20 @@
         <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -933,25 +920,25 @@
         <v>6</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -962,22 +949,22 @@
         <v>6</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>